<commit_message>
Updated the testing results as the use of one player improved from the baseline slightly in all parameters
</commit_message>
<xml_diff>
--- a/VRPHons/results/testing of simple system.xlsx
+++ b/VRPHons/results/testing of simple system.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
   <si>
     <t>blon-1</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>One Player</t>
+  </si>
+  <si>
+    <t>&lt;- All round improvement</t>
   </si>
 </sst>
 </file>
@@ -89,15 +92,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -105,14 +114,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -128,6 +177,66 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="http://puu.sh/skg2H/2138da6dd5.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8486775" y="800100"/>
+          <a:ext cx="6962775" cy="3895725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -427,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,7 +547,7 @@
     <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -470,42 +579,42 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>10</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <v>110</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <v>1955.1533350469099</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="4">
         <v>635.18583209599899</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="4">
         <v>5300.841107104</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="4">
         <v>790.33223732900001</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="4">
         <v>5</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -540,7 +649,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -573,10 +682,49 @@
       </c>
       <c r="K4" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>110</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1935.26403888302</v>
+      </c>
+      <c r="E5" s="1">
+        <v>630.14734060299998</v>
+      </c>
+      <c r="F5" s="1">
+        <v>5213.4013762690001</v>
+      </c>
+      <c r="G5" s="1">
+        <v>755.79354359700005</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reward information and updated overview of all visits
</commit_message>
<xml_diff>
--- a/VRPHons/results/testing of simple system.xlsx
+++ b/VRPHons/results/testing of simple system.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
     <t>blon-1</t>
   </si>
@@ -68,7 +68,10 @@
     <t>One Player</t>
   </si>
   <si>
-    <t>&lt;- All round improvement</t>
+    <t>&lt;- With look ahead</t>
+  </si>
+  <si>
+    <t>&lt;- Without look ahead</t>
   </si>
 </sst>
 </file>
@@ -155,13 +158,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -183,16 +196,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>554272</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -201,7 +214,7 @@
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill>
+      <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
@@ -209,15 +222,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect l="1368" t="2690" r="39398" b="2690"/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="8486775" y="800100"/>
-          <a:ext cx="6962775" cy="3895725"/>
+          <a:off x="10144125" y="209551"/>
+          <a:ext cx="2706921" cy="2419350"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -234,6 +245,138 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>542926</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>46963</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10153650" y="2619374"/>
+          <a:ext cx="2686050" cy="2418689"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8534400" y="923925"/>
+          <a:ext cx="1390650" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8153400" y="1123950"/>
+          <a:ext cx="1933575" cy="1676400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -536,14 +679,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -557,16 +702,16 @@
       <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="5" t="s">
         <v>8</v>
       </c>
       <c r="H1" t="s">
@@ -580,37 +725,37 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="2">
         <v>10</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="2">
         <v>110</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="6">
         <v>1955.1533350469099</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="6">
         <v>635.18583209599899</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="6">
         <v>5300.841107104</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="6">
         <v>790.33223732900001</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="2">
         <v>5</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -624,16 +769,16 @@
       <c r="C3">
         <v>110</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="5">
         <v>1961.08827481244</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="4">
         <v>626.45244678999995</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="4">
         <v>5278.9229001040003</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="4">
         <v>781.67454558199995</v>
       </c>
       <c r="H3">
@@ -659,16 +804,16 @@
       <c r="C4">
         <v>110</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="7">
         <v>1957.6034638696799</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="4">
         <v>634.17813379299901</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="5">
         <v>5306.0805300649999</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="5">
         <v>792.40180939499896</v>
       </c>
       <c r="H4">
@@ -694,16 +839,16 @@
       <c r="C5">
         <v>110</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="4">
         <v>1935.26403888302</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="4">
         <v>630.14734060299998</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="4">
         <v>5213.4013762690001</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="4">
         <v>755.79354359700005</v>
       </c>
       <c r="H5">
@@ -719,6 +864,44 @@
         <v>13</v>
       </c>
       <c r="L5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>110</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1857.93861354659</v>
+      </c>
+      <c r="E6" s="4">
+        <v>587.48811231099899</v>
+      </c>
+      <c r="F6" s="4">
+        <v>5059.290667108</v>
+      </c>
+      <c r="G6" s="4">
+        <v>694.91981350599997</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bid Altering (with suggestion and limit), Initial Balance set to 0, updated GUI (including time frame, indication when waiting)
</commit_message>
<xml_diff>
--- a/VRPHons/results/testing of simple system.xlsx
+++ b/VRPHons/results/testing of simple system.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
   <si>
     <t>blon-1</t>
   </si>
@@ -72,13 +72,16 @@
   </si>
   <si>
     <t>&lt;- Without look ahead</t>
+  </si>
+  <si>
+    <t>&lt;- Adjustable Bids</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +92,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -158,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -175,6 +186,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -679,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,6 +917,44 @@
         <v>14</v>
       </c>
     </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>110</v>
+      </c>
+      <c r="D7" s="8">
+        <v>1850.04780660353</v>
+      </c>
+      <c r="E7" s="8">
+        <v>525.34671678699999</v>
+      </c>
+      <c r="F7" s="8">
+        <v>5105.9822323259996</v>
+      </c>
+      <c r="G7" s="8">
+        <v>713.36298178599998</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>